<commit_message>
Update: Network_Config_Unified.xlsx uses simplified storage modes
Changed 6130 from 'both' to 'ambient' in example file.

All nodes now use frozen OR ambient only (no 'both').
Product states (frozen/ambient/thawed) handled via state transitions.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/examples/Network_Config_Unified.xlsx
+++ b/data/examples/Network_Config_Unified.xlsx
@@ -510,9 +510,6 @@
           <t>ambient</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v/>
-      </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
@@ -540,9 +537,6 @@
       <c r="C3" t="b">
         <v>0</v>
       </c>
-      <c r="D3" t="n">
-        <v/>
-      </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
@@ -581,9 +575,6 @@
       <c r="C4" t="b">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
-        <v/>
-      </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
@@ -622,9 +613,6 @@
       <c r="C5" t="b">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
-        <v/>
-      </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
@@ -663,9 +651,6 @@
       <c r="C6" t="b">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
-        <v/>
-      </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
@@ -673,9 +658,6 @@
         <is>
           <t>ambient</t>
         </is>
-      </c>
-      <c r="G6" t="n">
-        <v/>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -704,9 +686,6 @@
       <c r="C7" t="b">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
-        <v/>
-      </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
@@ -714,9 +693,6 @@
         <is>
           <t>ambient</t>
         </is>
-      </c>
-      <c r="G7" t="n">
-        <v/>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -745,9 +721,6 @@
       <c r="C8" t="b">
         <v>0</v>
       </c>
-      <c r="D8" t="n">
-        <v/>
-      </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
@@ -755,9 +728,6 @@
         <is>
           <t>ambient</t>
         </is>
-      </c>
-      <c r="G8" t="n">
-        <v/>
       </c>
       <c r="H8" t="b">
         <v>1</v>
@@ -786,9 +756,6 @@
       <c r="C9" t="b">
         <v>0</v>
       </c>
-      <c r="D9" t="n">
-        <v/>
-      </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
@@ -796,9 +763,6 @@
         <is>
           <t>ambient</t>
         </is>
-      </c>
-      <c r="G9" t="n">
-        <v/>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -827,9 +791,6 @@
       <c r="C10" t="b">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
-        <v/>
-      </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
@@ -837,9 +798,6 @@
         <is>
           <t>ambient</t>
         </is>
-      </c>
-      <c r="G10" t="n">
-        <v/>
       </c>
       <c r="H10" t="b">
         <v>1</v>
@@ -868,19 +826,13 @@
       <c r="C11" t="b">
         <v>0</v>
       </c>
-      <c r="D11" t="n">
-        <v/>
-      </c>
       <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>both</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v/>
+          <t>ambient</t>
+        </is>
       </c>
       <c r="H11" t="b">
         <v>1</v>
@@ -2195,9 +2147,6 @@
       <c r="D2" t="n">
         <v>37.5</v>
       </c>
-      <c r="E2" t="n">
-        <v/>
-      </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
@@ -2218,9 +2167,6 @@
       <c r="D3" t="n">
         <v>37.5</v>
       </c>
-      <c r="E3" t="n">
-        <v/>
-      </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
@@ -2241,9 +2187,6 @@
       <c r="D4" t="n">
         <v>37.5</v>
       </c>
-      <c r="E4" t="n">
-        <v/>
-      </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
@@ -2310,9 +2253,6 @@
       <c r="D7" t="n">
         <v>37.5</v>
       </c>
-      <c r="E7" t="n">
-        <v/>
-      </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
@@ -2333,9 +2273,6 @@
       <c r="D8" t="n">
         <v>37.5</v>
       </c>
-      <c r="E8" t="n">
-        <v/>
-      </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
@@ -2356,9 +2293,6 @@
       <c r="D9" t="n">
         <v>37.5</v>
       </c>
-      <c r="E9" t="n">
-        <v/>
-      </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
@@ -2379,9 +2313,6 @@
       <c r="D10" t="n">
         <v>37.5</v>
       </c>
-      <c r="E10" t="n">
-        <v/>
-      </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
@@ -2402,9 +2333,6 @@
       <c r="D11" t="n">
         <v>37.5</v>
       </c>
-      <c r="E11" t="n">
-        <v/>
-      </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
@@ -2471,9 +2399,6 @@
       <c r="D14" t="n">
         <v>37.5</v>
       </c>
-      <c r="E14" t="n">
-        <v/>
-      </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
@@ -2494,9 +2419,6 @@
       <c r="D15" t="n">
         <v>37.5</v>
       </c>
-      <c r="E15" t="n">
-        <v/>
-      </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
@@ -2517,9 +2439,6 @@
       <c r="D16" t="n">
         <v>37.5</v>
       </c>
-      <c r="E16" t="n">
-        <v/>
-      </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
@@ -2540,9 +2459,6 @@
       <c r="D17" t="n">
         <v>37.5</v>
       </c>
-      <c r="E17" t="n">
-        <v/>
-      </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
@@ -2563,9 +2479,6 @@
       <c r="D18" t="n">
         <v>37.5</v>
       </c>
-      <c r="E18" t="n">
-        <v/>
-      </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
@@ -2632,9 +2545,6 @@
       <c r="D21" t="n">
         <v>37.5</v>
       </c>
-      <c r="E21" t="n">
-        <v/>
-      </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
@@ -2655,9 +2565,6 @@
       <c r="D22" t="n">
         <v>37.5</v>
       </c>
-      <c r="E22" t="n">
-        <v/>
-      </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
@@ -2678,9 +2585,6 @@
       <c r="D23" t="n">
         <v>37.5</v>
       </c>
-      <c r="E23" t="n">
-        <v/>
-      </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
@@ -2701,9 +2605,6 @@
       <c r="D24" t="n">
         <v>37.5</v>
       </c>
-      <c r="E24" t="n">
-        <v/>
-      </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
@@ -2724,9 +2625,6 @@
       <c r="D25" t="n">
         <v>37.5</v>
       </c>
-      <c r="E25" t="n">
-        <v/>
-      </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
@@ -2793,9 +2691,6 @@
       <c r="D28" t="n">
         <v>37.5</v>
       </c>
-      <c r="E28" t="n">
-        <v/>
-      </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
@@ -2816,9 +2711,6 @@
       <c r="D29" t="n">
         <v>37.5</v>
       </c>
-      <c r="E29" t="n">
-        <v/>
-      </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
@@ -2839,9 +2731,6 @@
       <c r="D30" t="n">
         <v>37.5</v>
       </c>
-      <c r="E30" t="n">
-        <v/>
-      </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
@@ -2861,9 +2750,6 @@
       </c>
       <c r="D31" t="n">
         <v>37.5</v>
-      </c>
-      <c r="E31" t="n">
-        <v/>
       </c>
       <c r="F31" t="n">
         <v>0</v>

</xml_diff>